<commit_message>
Por alguna razon, hay un problema con los dataframes de las interacciones. Dice que no existe un par cuando si existe. Por ejemplo, no encuentra un stop para un start. Haces debug y si existe. Hay algo en el formato que provoca que piense que no es igual
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/results.xlsx
+++ b/data_analysis/db_env/app/results/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,70 +456,90 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>TD</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>GP_N</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>GP_T</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>GP_T_SC</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>OI_N</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>OI_N_type_1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>OI_N_type_2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>OI_N_type_3</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>OI_N_type_4</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OI_N_actor_2</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>OI_N_actor_3</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OI_N_actor_4</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>OI_N_actor_5</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>OI_N_actor_10</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>OI_N_actor_11</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>OI_T</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>OI_T_SS</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>OI_T_GR</t>
         </is>
@@ -550,46 +570,58 @@
         </is>
       </c>
       <c r="F2" t="n">
+        <v>1433.02</v>
+      </c>
+      <c r="G2" t="n">
+        <v>24</v>
+      </c>
+      <c r="H2" t="n">
+        <v>57.91</v>
+      </c>
+      <c r="I2" t="n">
+        <v>49.55</v>
+      </c>
+      <c r="J2" t="n">
         <v>149</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>49</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
         <v>49</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>26</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>25</v>
       </c>
-      <c r="K2" t="n">
+      <c r="O2" t="n">
         <v>42</v>
       </c>
-      <c r="L2" t="n">
+      <c r="P2" t="n">
         <v>36</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q2" t="n">
         <v>24</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>33</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>2</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="U2" t="n">
         <v>8.74</v>
       </c>
-      <c r="R2" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="S2" t="n">
-        <v>-72.98</v>
+      <c r="V2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="W2" t="n">
+        <v>20.79</v>
       </c>
     </row>
     <row r="3">
@@ -617,46 +649,58 @@
         </is>
       </c>
       <c r="F3" t="n">
+        <v>282.26</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>47.28</v>
+      </c>
+      <c r="I3" t="n">
+        <v>45.36</v>
+      </c>
+      <c r="J3" t="n">
         <v>28</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
         <v>9</v>
       </c>
-      <c r="H3" t="n">
+      <c r="L3" t="n">
         <v>9</v>
       </c>
-      <c r="I3" t="n">
+      <c r="M3" t="n">
         <v>5</v>
       </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>5</v>
       </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
         <v>4</v>
       </c>
-      <c r="L3" t="n">
+      <c r="P3" t="n">
         <v>12</v>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
       <c r="Q3" t="n">
-        <v>3.04</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>2.4</v>
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2.07</v>
       </c>
     </row>
     <row r="4">
@@ -684,46 +728,58 @@
         </is>
       </c>
       <c r="F4" t="n">
+        <v>199.31</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>42.27</v>
+      </c>
+      <c r="I4" t="n">
+        <v>35.11</v>
+      </c>
+      <c r="J4" t="n">
         <v>58</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
         <v>19</v>
       </c>
-      <c r="H4" t="n">
+      <c r="L4" t="n">
         <v>19</v>
       </c>
-      <c r="I4" t="n">
+      <c r="M4" t="n">
         <v>10</v>
       </c>
-      <c r="J4" t="n">
+      <c r="N4" t="n">
         <v>10</v>
       </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
         <v>30</v>
       </c>
-      <c r="L4" t="n">
+      <c r="P4" t="n">
         <v>16</v>
       </c>
-      <c r="M4" t="n">
+      <c r="Q4" t="n">
         <v>12</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1.53</v>
-      </c>
       <c r="R4" t="n">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>-4</v>
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="W4" t="n">
+        <v>4.6</v>
       </c>
     </row>
     <row r="5">
@@ -751,46 +807,58 @@
         </is>
       </c>
       <c r="F5" t="n">
+        <v>385.14</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>68.02</v>
+      </c>
+      <c r="I5" t="n">
+        <v>68.18000000000001</v>
+      </c>
+      <c r="J5" t="n">
         <v>22</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
         <v>8</v>
       </c>
-      <c r="H5" t="n">
+      <c r="L5" t="n">
         <v>8</v>
       </c>
-      <c r="I5" t="n">
+      <c r="M5" t="n">
         <v>3</v>
       </c>
-      <c r="J5" t="n">
+      <c r="N5" t="n">
         <v>3</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>4</v>
       </c>
-      <c r="M5" t="n">
+      <c r="Q5" t="n">
         <v>4</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
         <v>12</v>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
         <v>2</v>
       </c>
-      <c r="Q5" t="n">
-        <v>6.81</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="S5" t="n">
-        <v>26</v>
+      <c r="U5" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="W5" t="n">
+        <v>21.21</v>
       </c>
     </row>
     <row r="6">
@@ -818,46 +886,60 @@
         </is>
       </c>
       <c r="F6" t="n">
+        <v>545.02</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9</v>
+      </c>
+      <c r="H6" t="n">
+        <v>43.86</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
         <v>41</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
         <v>13</v>
       </c>
-      <c r="H6" t="n">
+      <c r="L6" t="n">
         <v>13</v>
-      </c>
-      <c r="I6" t="n">
-        <v>8</v>
-      </c>
-      <c r="J6" t="n">
-        <v>7</v>
-      </c>
-      <c r="K6" t="n">
-        <v>8</v>
-      </c>
-      <c r="L6" t="n">
-        <v>4</v>
       </c>
       <c r="M6" t="n">
         <v>8</v>
       </c>
       <c r="N6" t="n">
+        <v>7</v>
+      </c>
+      <c r="O6" t="n">
+        <v>8</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>8</v>
+      </c>
+      <c r="R6" t="n">
         <v>21</v>
       </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>10.35</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.27</v>
-      </c>
       <c r="S6" t="n">
-        <v>47.9</v>
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="W6" t="n">
+        <v>47.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
He arreglado alguna cosilla de Unreal. Estaba ahora con NPCInteractionEvents. Me he dado cuenta que si no hay eventos de ese tipo en un escenario, pasan cosas raras con el excel final. Hay que hacer el concat de alguna manera que ahora mismo no me sale
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/results.xlsx
+++ b/data_analysis/db_env/app/results/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +544,61 @@
           <t>OI_T_GR</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_T</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_0</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_type_2</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_1</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_2</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_3</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_4</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_5</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_N_actor_6</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -576,10 +631,10 @@
         <v>24</v>
       </c>
       <c r="H2" t="n">
-        <v>57.91</v>
+        <v>57.914</v>
       </c>
       <c r="I2" t="n">
-        <v>49.55</v>
+        <v>49.515</v>
       </c>
       <c r="J2" t="n">
         <v>149</v>
@@ -615,13 +670,46 @@
         <v>2</v>
       </c>
       <c r="U2" t="n">
-        <v>8.74</v>
+        <v>8.734</v>
       </c>
       <c r="V2" t="n">
-        <v>0.45</v>
+        <v>0.29</v>
       </c>
       <c r="W2" t="n">
-        <v>20.79</v>
+        <v>19.885</v>
+      </c>
+      <c r="X2" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>76.73999999999999</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -655,10 +743,10 @@
         <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>47.28</v>
+        <v>47.284</v>
       </c>
       <c r="I3" t="n">
-        <v>45.36</v>
+        <v>45.364</v>
       </c>
       <c r="J3" t="n">
         <v>28</v>
@@ -694,13 +782,46 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>3.03</v>
+        <v>3.029</v>
       </c>
       <c r="V3" t="n">
-        <v>0.43</v>
+        <v>0.426</v>
       </c>
       <c r="W3" t="n">
         <v>2.07</v>
+      </c>
+      <c r="X3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>24.092</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -737,7 +858,7 @@
         <v>42.27</v>
       </c>
       <c r="I4" t="n">
-        <v>35.11</v>
+        <v>35.142</v>
       </c>
       <c r="J4" t="n">
         <v>58</v>
@@ -773,13 +894,46 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>1.52</v>
+        <v>1.525</v>
       </c>
       <c r="V4" t="n">
-        <v>0.16</v>
+        <v>0.194</v>
       </c>
       <c r="W4" t="n">
-        <v>4.6</v>
+        <v>5.356</v>
+      </c>
+      <c r="X4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>28.444</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -816,7 +970,7 @@
         <v>68.02</v>
       </c>
       <c r="I5" t="n">
-        <v>68.18000000000001</v>
+        <v>68.038</v>
       </c>
       <c r="J5" t="n">
         <v>22</v>
@@ -852,13 +1006,46 @@
         <v>2</v>
       </c>
       <c r="U5" t="n">
-        <v>6.8</v>
+        <v>6.797</v>
       </c>
       <c r="V5" t="n">
-        <v>0.5</v>
+        <v>0.408</v>
       </c>
       <c r="W5" t="n">
-        <v>21.21</v>
+        <v>21.225</v>
+      </c>
+      <c r="X5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>31.68</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -892,7 +1079,7 @@
         <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>43.86</v>
+        <v>43.862</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -933,13 +1120,68 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>10.36</v>
+        <v>10.351</v>
       </c>
       <c r="V6" t="n">
-        <v>0.37</v>
+        <v>0.287</v>
       </c>
       <c r="W6" t="n">
-        <v>47.96</v>
+        <v>47.836</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuo con el analisis. Ahora se crea un csv con los items y npcs que hay en cada escenario.
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/results.xlsx
+++ b/data_analysis/db_env/app/results/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,147 +456,72 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>TD</t>
+          <t>OI_N</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>GP_N</t>
+          <t>OI_N_type_1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>GP_T</t>
+          <t>OI_N_type_2</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>GP_T_SC</t>
+          <t>OI_N_type_3</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>OI_N</t>
+          <t>OI_N_type_4</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_1</t>
+          <t>OI_N_actor_2</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_2</t>
+          <t>OI_N_actor_3</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_3</t>
+          <t>OI_N_actor_4</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_4</t>
+          <t>OI_N_actor_5</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_actor_2</t>
+          <t>OI_N_actor_10</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_actor_3</t>
+          <t>OI_N_actor_11</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_actor_4</t>
+          <t>OI_T</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_actor_5</t>
+          <t>OI_T_SS</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_actor_10</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_11</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T_SS</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
           <t>OI_T_GR</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_T</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_type_0</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_type_1</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_type_2</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_actor_1</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_actor_2</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_actor_3</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_actor_4</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_actor_5</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>NPC_N_actor_6</t>
         </is>
       </c>
     </row>
@@ -625,91 +550,46 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1433.02</v>
+        <v>149</v>
       </c>
       <c r="G2" t="n">
+        <v>49</v>
+      </c>
+      <c r="H2" t="n">
+        <v>49</v>
+      </c>
+      <c r="I2" t="n">
+        <v>26</v>
+      </c>
+      <c r="J2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K2" t="n">
+        <v>42</v>
+      </c>
+      <c r="L2" t="n">
+        <v>36</v>
+      </c>
+      <c r="M2" t="n">
         <v>24</v>
       </c>
-      <c r="H2" t="n">
-        <v>57.914</v>
-      </c>
-      <c r="I2" t="n">
-        <v>49.515</v>
-      </c>
-      <c r="J2" t="n">
-        <v>149</v>
-      </c>
-      <c r="K2" t="n">
-        <v>49</v>
-      </c>
-      <c r="L2" t="n">
-        <v>49</v>
-      </c>
-      <c r="M2" t="n">
-        <v>26</v>
-      </c>
       <c r="N2" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="O2" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="Q2" t="n">
-        <v>24</v>
+        <v>8.734</v>
       </c>
       <c r="R2" t="n">
-        <v>33</v>
+        <v>0.29</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>2</v>
-      </c>
-      <c r="U2" t="n">
-        <v>8.734</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="W2" t="n">
         <v>19.885</v>
-      </c>
-      <c r="X2" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>76.73999999999999</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>7</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>6</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -737,91 +617,46 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>282.26</v>
+        <v>28</v>
       </c>
       <c r="G3" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" t="n">
         <v>5</v>
       </c>
-      <c r="H3" t="n">
-        <v>47.284</v>
-      </c>
-      <c r="I3" t="n">
-        <v>45.364</v>
-      </c>
       <c r="J3" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="K3" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L3" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="M3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>3.029</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>0.426</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>3.029</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.426</v>
-      </c>
-      <c r="W3" t="n">
         <v>2.07</v>
-      </c>
-      <c r="X3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>24.092</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -849,91 +684,46 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>199.31</v>
+        <v>58</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H4" t="n">
-        <v>42.27</v>
+        <v>19</v>
       </c>
       <c r="I4" t="n">
-        <v>35.142</v>
+        <v>10</v>
       </c>
       <c r="J4" t="n">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="K4" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="L4" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>12</v>
+        <v>1.525</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.194</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>1.525</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.194</v>
-      </c>
-      <c r="W4" t="n">
         <v>5.356</v>
-      </c>
-      <c r="X4" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>28.444</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -961,91 +751,46 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>385.14</v>
+        <v>22</v>
       </c>
       <c r="G5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H5" t="n">
-        <v>68.02</v>
+        <v>8</v>
       </c>
       <c r="I5" t="n">
-        <v>68.038</v>
+        <v>3</v>
       </c>
       <c r="J5" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="K5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N5" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q5" t="n">
-        <v>4</v>
+        <v>6.797</v>
       </c>
       <c r="R5" t="n">
-        <v>12</v>
+        <v>0.408</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
-        <v>2</v>
-      </c>
-      <c r="U5" t="n">
-        <v>6.797</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.408</v>
-      </c>
-      <c r="W5" t="n">
         <v>21.225</v>
-      </c>
-      <c r="X5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>31.68</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -1073,115 +818,46 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>545.02</v>
+        <v>41</v>
       </c>
       <c r="G6" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H6" t="n">
-        <v>43.862</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="I6" t="n">
+        <v>8</v>
       </c>
       <c r="J6" t="n">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="K6" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L6" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
         <v>8</v>
       </c>
       <c r="N6" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="O6" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>8</v>
+        <v>10.351</v>
       </c>
       <c r="R6" t="n">
-        <v>21</v>
+        <v>0.287</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>10.351</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.287</v>
-      </c>
-      <c r="W6" t="n">
         <v>47.836</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>NULL</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadidos los datos del usuario AB.
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/results.xlsx
+++ b/data_analysis/db_env/app/results/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,72 +456,22 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>OI_N</t>
+          <t>TD</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_1</t>
+          <t>GP_N</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_2</t>
+          <t>GP_T</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>OI_N_type_3</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_type_4</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_2</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_3</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_4</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_5</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_10</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>OI_N_actor_11</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T_SS</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>OI_T_GR</t>
+          <t>GP_T_SC</t>
         </is>
       </c>
     </row>
@@ -550,46 +500,16 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>149</v>
+        <v>1433.02</v>
       </c>
       <c r="G2" t="n">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="H2" t="n">
-        <v>49</v>
+        <v>57.914</v>
       </c>
       <c r="I2" t="n">
-        <v>26</v>
-      </c>
-      <c r="J2" t="n">
-        <v>25</v>
-      </c>
-      <c r="K2" t="n">
-        <v>42</v>
-      </c>
-      <c r="L2" t="n">
-        <v>36</v>
-      </c>
-      <c r="M2" t="n">
-        <v>24</v>
-      </c>
-      <c r="N2" t="n">
-        <v>33</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>8.734</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="S2" t="n">
-        <v>19.885</v>
+        <v>52.486875</v>
       </c>
     </row>
     <row r="3">
@@ -617,46 +537,16 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>28</v>
+        <v>282.26</v>
       </c>
       <c r="G3" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>9</v>
+        <v>47.284</v>
       </c>
       <c r="I3" t="n">
-        <v>5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>5</v>
-      </c>
-      <c r="K3" t="n">
-        <v>4</v>
-      </c>
-      <c r="L3" t="n">
-        <v>12</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>3.029</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.426</v>
-      </c>
-      <c r="S3" t="n">
-        <v>2.07</v>
+        <v>45.364</v>
       </c>
     </row>
     <row r="4">
@@ -684,46 +574,16 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>58</v>
+        <v>199.31</v>
       </c>
       <c r="G4" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="H4" t="n">
-        <v>19</v>
+        <v>42.27</v>
       </c>
       <c r="I4" t="n">
-        <v>10</v>
-      </c>
-      <c r="J4" t="n">
-        <v>10</v>
-      </c>
-      <c r="K4" t="n">
-        <v>30</v>
-      </c>
-      <c r="L4" t="n">
-        <v>16</v>
-      </c>
-      <c r="M4" t="n">
-        <v>12</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1.525</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.194</v>
-      </c>
-      <c r="S4" t="n">
-        <v>5.356</v>
+        <v>35.1424</v>
       </c>
     </row>
     <row r="5">
@@ -751,46 +611,16 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>22</v>
+        <v>385.14</v>
       </c>
       <c r="G5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H5" t="n">
-        <v>8</v>
+        <v>68.02</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>12</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>6.797</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.408</v>
-      </c>
-      <c r="S5" t="n">
-        <v>21.225</v>
+        <v>68.0376</v>
       </c>
     </row>
     <row r="6">
@@ -818,46 +648,201 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>41</v>
+        <v>545.02</v>
       </c>
       <c r="G6" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>13</v>
+        <v>43.862</v>
       </c>
       <c r="I6" t="n">
+        <v>57.44055555555556</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>QUEST</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1236.99</v>
+      </c>
+      <c r="G7" t="n">
+        <v>24</v>
+      </c>
+      <c r="H7" t="n">
+        <v>49.323</v>
+      </c>
+      <c r="I7" t="n">
+        <v>43.423375</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>QUEST</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>230.1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>35.78</v>
+      </c>
+      <c r="I8" t="n">
+        <v>34.9544</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>QUEST</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>197.1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>41.622</v>
+      </c>
+      <c r="I9" t="n">
+        <v>34.7066</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="J6" t="n">
-        <v>7</v>
-      </c>
-      <c r="K6" t="n">
-        <v>8</v>
-      </c>
-      <c r="L6" t="n">
-        <v>4</v>
-      </c>
-      <c r="M6" t="n">
-        <v>8</v>
-      </c>
-      <c r="N6" t="n">
-        <v>21</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>10.351</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.287</v>
-      </c>
-      <c r="S6" t="n">
-        <v>47.836</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>QUEST</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>298.34</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>53.045</v>
+      </c>
+      <c r="I10" t="n">
+        <v>48.6206</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CTRL</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>QUEST</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>486.41</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" t="n">
+        <v>38.522</v>
+      </c>
+      <c r="I11" t="n">
+        <v>50.08366666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>